<commit_message>
Sprint-1: Week-1 :- Updated repository
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeapThoughtProjectWS\FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="121">
   <si>
     <t>textbox</t>
   </si>
@@ -289,6 +289,105 @@
   </si>
   <si>
     <t>Fulcrum Component</t>
+  </si>
+  <si>
+    <t>Ribbon.Documents.New.AT.CompleteAction-Large</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Ribbon.Documents.New.AT.AttachDocument-Large</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Attach Document</t>
+  </si>
+  <si>
+    <t>Ribbon.Documents.New.AT.AttachSupportDocument-Large</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Attach Support Document</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Document Registry</t>
+  </si>
+  <si>
+    <t>selectitembytextfromlist</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'docLibList')]/li/a</t>
+  </si>
+  <si>
+    <t>Attach Documents Window</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Attach</t>
+  </si>
+  <si>
+    <t>.//*[@class='attach-button']</t>
+  </si>
+  <si>
+    <t>.//*[@id='divTransmittalFiles']/ul/li[contains(text(),'docName')]</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Attached Transmittal Files</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Attached Support Document Files</t>
+  </si>
+  <si>
+    <t>.//*[@id='divSupportingFiles']/ul/li[contains(text(),'docName')]</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Attached Review Document Files</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Attach Review Sheet</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Edit</t>
+  </si>
+  <si>
+    <t>Ribbon.ListForm.Edit-title</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View -Transmittal Files</t>
+  </si>
+  <si>
+    <t>.//*[@id='transmittalFiles']/descendant :: span/a[text()='docName']</t>
+  </si>
+  <si>
+    <t>.//*[@id='supportingDocumentFiles']/descendant :: span/a[text()='docName']</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View -Supporting Document Files</t>
+  </si>
+  <si>
+    <t>.//*[@id='onetidIOFile']</t>
+  </si>
+  <si>
+    <t>Ribbon.ListItem.Actions.AttachReviewSheetFile-Large</t>
+  </si>
+  <si>
+    <t>attachOKbutton</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Browse-OK</t>
+  </si>
+  <si>
+    <t>.//*[@id='idAttachmentsTable']/descendant :: span[contains(text(),'docName')]</t>
+  </si>
+  <si>
+    <t>View Page</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View - Attached Review Document Files</t>
+  </si>
+  <si>
+    <t>.//*[@class='DocRegisterLinks reviewSheetLnks']/li/a[contains(text(),'docName')]</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Browse</t>
   </si>
 </sst>
 </file>
@@ -380,10 +479,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,11 +829,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A32"/>
+  <dimension ref="A2:A33"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
-    </sheetView>
+    <sheetView topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -894,6 +991,11 @@
     <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -910,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -921,7 +1023,7 @@
     <col min="2" max="2" width="44.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="5" max="5" width="52.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -949,15 +1051,15 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
@@ -1047,38 +1149,38 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1170,15 +1272,15 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
@@ -1252,11 +1354,128 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="E40" s="4"/>
+    <row r="23" spans="1:9">
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="E41" s="4"/>
@@ -1264,48 +1483,55 @@
     <row r="42" spans="1:7">
       <c r="E42" s="4"/>
     </row>
+    <row r="43" spans="1:7">
+      <c r="E43" s="4"/>
+    </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="E44" s="4"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A31:G31"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C48 C51 C18:C43 C45:C46 C3:C16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C50 C53 C3:C16 C47:C48 C32:C45 C18:C30">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1319,7 +1545,7 @@
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$39</xm:f>
           </x14:formula1>
-          <xm:sqref>D43 D45:D46 D18:D33 D48 D51 D3:D16</xm:sqref>
+          <xm:sqref>D45 D47:D48 D3:D16 D50 D53 D32:D35 D18:D30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1329,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1340,7 +1566,7 @@
     <col min="2" max="2" width="44.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1368,31 +1594,34 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:9">
       <c r="B3" t="s">
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="G3" t="s">
         <v>60</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1409,71 +1638,157 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+    <row r="5" spans="1:9">
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:7">
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:7">
-      <c r="E37" s="4"/>
-    </row>
     <row r="38" spans="1:7">
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="E39" s="4"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A38:G38"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A47:G47"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C45 C48 C16:C40 C42:C43 C3:C14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C42 C45 C39:C40 C13:C14 C16:C37 C3:C8 C11">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1487,7 +1802,7 @@
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$39</xm:f>
           </x14:formula1>
-          <xm:sqref>D40 D42:D43 D16:D30 D45 D48 D3:D14</xm:sqref>
+          <xm:sqref>D37 D39:D40 D42 D45 D13:D14 D16:D27 D3:D8 D11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Included elements for Cancel and Close transmittals(enable/disable)
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="132">
   <si>
     <t>textbox</t>
   </si>
@@ -243,9 +243,6 @@
     <t>(.//*[@value='Submit'])[2]</t>
   </si>
   <si>
-    <t>Tramsmittals-View -Cancel</t>
-  </si>
-  <si>
     <t>Tramsmittals-Close Dialog</t>
   </si>
   <si>
@@ -388,6 +385,42 @@
   </si>
   <si>
     <t>Tramsmittals-Browse</t>
+  </si>
+  <si>
+    <t>element_enable</t>
+  </si>
+  <si>
+    <t>element_disable</t>
+  </si>
+  <si>
+    <t>element_displayed</t>
+  </si>
+  <si>
+    <t>element_notdisplayed</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View -Cancel - IsEnabled</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View -Cancel - IsDisabled</t>
+  </si>
+  <si>
+    <t>Ribbon.ListForm.Display.Respond.Cancel-Medium</t>
+  </si>
+  <si>
+    <t>Ribbon.Documents.New.AT.CloseTransmittal-Large</t>
+  </si>
+  <si>
+    <t>Tramsmittals-Close Transmittal</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View -Close Transmittal - IsEnabled</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View -Close Transmittal - IsDisabled</t>
+  </si>
+  <si>
+    <t>element_disable_attribute</t>
   </si>
 </sst>
 </file>
@@ -829,9 +862,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A33"/>
+  <dimension ref="A2:A38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -990,12 +1025,37 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1012,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1072,7 +1132,7 @@
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1139,10 +1199,10 @@
         <v>35</v>
       </c>
       <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" t="s">
         <v>75</v>
-      </c>
-      <c r="E8" t="s">
-        <v>76</v>
       </c>
       <c r="G8" t="s">
         <v>59</v>
@@ -1156,19 +1216,19 @@
         <v>35</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>35</v>
@@ -1177,11 +1237,11 @@
         <v>16</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1206,10 +1266,10 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
         <v>51</v>
@@ -1259,7 +1319,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -1268,7 +1328,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1295,7 +1355,7 @@
         <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1342,21 +1402,21 @@
     </row>
     <row r="22" spans="1:9">
       <c r="B22" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="B23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
@@ -1370,49 +1430,49 @@
     </row>
     <row r="24" spans="1:9">
       <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
         <v>111</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="B25" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
         <v>115</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="B27" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -1421,7 +1481,7 @@
         <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1435,47 +1495,96 @@
         <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="B29" t="s">
         <v>102</v>
       </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
         <v>21</v>
       </c>
-      <c r="E29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="E31" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="B32" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" t="s">
-        <v>119</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="E32" t="str">
+        <f>Objects_Transmittals_Toolbar!E9</f>
+        <v>Ribbon.ListForm.Display.Respond.Cancel-Medium</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="B33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" t="str">
+        <f>E32</f>
+        <v>Ribbon.ListForm.Display.Respond.Cancel-Medium</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" t="str">
+        <f>Objects_Transmittals_Toolbar!E10</f>
+        <v>Ribbon.Documents.New.AT.CloseTransmittal-Large</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="B35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" t="str">
+        <f>E34</f>
+        <v>Ribbon.Documents.New.AT.CloseTransmittal-Large</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:7">
       <c r="E41" s="4"/>
@@ -1486,52 +1595,49 @@
     <row r="43" spans="1:7">
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:7">
-      <c r="E44" s="4"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+    <row r="45" spans="1:7">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A30:G30"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C50 C53 C3:C16 C47:C48 C32:C45 C18:C30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C49 C52 C3:C16 C46:C47 C18:C29 C31:C44">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1543,9 +1649,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Objects!$A$2:$A$39</xm:f>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>D45 D47:D48 D3:D16 D50 D53 D32:D35 D18:D30</xm:sqref>
+          <xm:sqref>D44 D46:D47 D52 D49 D3:D16 D18:D29 D31:D35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1558,7 +1664,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1566,7 +1672,7 @@
     <col min="2" max="2" width="44.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1609,24 +1715,24 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
         <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1635,68 +1741,96 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1709,21 +1843,21 @@
     </row>
     <row r="13" spans="1:9">
       <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
         <v>94</v>
       </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>95</v>
-      </c>
-      <c r="E13" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
@@ -1732,7 +1866,7 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1788,7 +1922,7 @@
     <mergeCell ref="A44:G44"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C42 C45 C39:C40 C13:C14 C16:C37 C3:C8 C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C42 C45 C39:C40 C13:C14 C16:C37 C3:C11">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1797,12 +1931,54 @@
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Objects!$A$2:$A$39</xm:f>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>D37 D39:D40 D42 D45 D13:D14 D16:D27 D3:D8 D11</xm:sqref>
+          <xm:sqref>D37</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D39:D40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D42</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D45</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D13:D14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D16:D27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Included Reply All objects
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,9 +16,6 @@
     <sheet name="Objects_Transmittals" sheetId="2" r:id="rId2"/>
     <sheet name="Objects_Transmittals_Toolbar" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Objects_Transmittals!$A$1:$G$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Objects_Transmittals_Toolbar!$A$1:$G$10</definedName>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="133">
   <si>
     <t>textbox</t>
   </si>
@@ -210,9 +207,6 @@
     <t>.//*[@id='TransmittalType_$containereditableRegion']</t>
   </si>
   <si>
-    <t>.//*[@alt='Complete Action']</t>
-  </si>
-  <si>
     <t>Tramsmittals-Complete Action</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>Tramsmittals-Close Dialog</t>
   </si>
   <si>
-    <t>.//*[text()='You have an open action. Complete Action']</t>
-  </si>
-  <si>
     <t>textbox_autosuggest_browse</t>
   </si>
   <si>
@@ -432,7 +423,7 @@
     <t>(.//span[contains(@id,'TransmittalTo_')])[5]</t>
   </si>
   <si>
-    <t>.//*[@class='ms-cui-ctl-mediumlabel' and text() = 'Reply All']</t>
+    <t>Ribbon.ListForm.Display.Respond.ReplyAll-Medium</t>
   </si>
 </sst>
 </file>
@@ -543,23 +534,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Objects"/>
-      <sheetName val="Objects_Transmittals"/>
-      <sheetName val="Objects_Transmittals_Toolbar"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1054,37 +1028,37 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1101,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1152,7 +1126,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -1161,7 +1135,7 @@
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1228,10 +1202,10 @@
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
         <v>59</v>
@@ -1245,19 +1219,19 @@
         <v>35</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>35</v>
@@ -1266,11 +1240,11 @@
         <v>16</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1295,10 +1269,10 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" t="s">
         <v>51</v>
@@ -1348,7 +1322,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -1357,12 +1331,12 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1375,7 +1349,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -1384,12 +1358,12 @@
         <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="B19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
@@ -1398,12 +1372,12 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="B20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
@@ -1412,12 +1386,12 @@
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="B21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
@@ -1426,12 +1400,12 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="B22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
@@ -1440,12 +1414,12 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="B23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
@@ -1454,12 +1428,12 @@
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="B24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
@@ -1468,26 +1442,26 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="B25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="B26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
@@ -1496,12 +1470,12 @@
         <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="B27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -1510,12 +1484,12 @@
         <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="B28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
@@ -1524,12 +1498,12 @@
         <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="B29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
@@ -1538,93 +1512,96 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>133</v>
-      </c>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="6" t="s">
+      <c r="B31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:9">
       <c r="B32" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" t="s">
         <v>118</v>
+      </c>
+      <c r="E32" t="str">
+        <f>Objects_Transmittals_Toolbar!E9</f>
+        <v>Ribbon.ListForm.Display.Respond.Cancel-Medium</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D33" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E33" t="str">
-        <f>Objects_Transmittals_Toolbar!E9</f>
+        <f>E32</f>
         <v>Ribbon.ListForm.Display.Respond.Cancel-Medium</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D34" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E34" t="str">
-        <f>E33</f>
-        <v>Ribbon.ListForm.Display.Respond.Cancel-Medium</v>
+        <f>Objects_Transmittals_Toolbar!E10</f>
+        <v>Ribbon.Documents.New.AT.CloseTransmittal-Large</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" t="s">
         <v>129</v>
       </c>
-      <c r="C35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" t="s">
-        <v>120</v>
-      </c>
       <c r="E35" t="str">
-        <f>Objects_Transmittals_Toolbar!E10</f>
+        <f>E34</f>
         <v>Ribbon.Documents.New.AT.CloseTransmittal-Large</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="B36" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E36" t="str">
-        <f>E35</f>
-        <v>Ribbon.Documents.New.AT.CloseTransmittal-Large</v>
-      </c>
+    <row r="40" spans="1:7">
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:7">
       <c r="E41" s="4"/>
@@ -1635,52 +1612,49 @@
     <row r="43" spans="1:7">
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:7">
-      <c r="E44" s="4"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+    <row r="45" spans="1:7">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A30:G30"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C50 C53 C3:C16 C47:C48 C32:C45 C18:C30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C49 C52 C3:C16 C46:C47 C31:C44 C18:C29">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1689,18 +1663,12 @@
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>D45 D47:D48 D53 D50 D3:D16 D32:D36 D18:D28 D30</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Objects!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D29</xm:sqref>
+          <xm:sqref>D44 D46:D47 D52 D49 D3:D16 D31:D35 D18:D28 D29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1710,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1750,7 +1718,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1761,27 +1729,21 @@
     </row>
     <row r="3" spans="1:9">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1790,63 +1752,63 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="B8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1854,83 +1816,86 @@
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="B10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="B11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
-      </c>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="B15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>98</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:7">
       <c r="E34" s="4"/>
@@ -1941,51 +1906,48 @@
     <row r="36" spans="1:7">
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:7">
-      <c r="E37" s="4"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+    <row r="38" spans="1:7">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A44:G44"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C43 C46 C40:C41 C14:C15 C17:C38 C3:C10 C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C42 C45 C39:C40 C13:C14 C16:C37 C3:C10 C11">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1999,7 +1961,7 @@
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>D38 D40:D41 D17:D28 D14:D15 D46 D43 D3:D10 D12</xm:sqref>
+          <xm:sqref>D37 D39:D40 D16:D27 D13:D14 D45 D42 D3:D10 D11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Included BUTTON_SCROLLABLE object type and mapped to send.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
@@ -5,11 +5,11 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" state="hidden" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="138">
   <si>
     <t>textbox</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>(.//span[contains(@id,'AssignedTo_')])[1]</t>
+  </si>
+  <si>
+    <t>button_scrollable</t>
   </si>
 </sst>
 </file>
@@ -877,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A38"/>
+  <dimension ref="A2:A39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1071,6 +1074,11 @@
     <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1089,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1312,7 +1320,7 @@
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>137</v>
       </c>
       <c r="E14" t="s">
         <v>56</v>
@@ -1703,12 +1711,48 @@
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Objects!$A$2:$A$38</xm:f>
+            <xm:f>Objects!$A$2:$A$99</xm:f>
           </x14:formula1>
-          <xm:sqref>D46 D48:D49 D54 D51 D3:D16 D33:D37 D18:D31</xm:sqref>
+          <xm:sqref>D46</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$99</xm:f>
+          </x14:formula1>
+          <xm:sqref>D48:D49</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$99</xm:f>
+          </x14:formula1>
+          <xm:sqref>D54</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$99</xm:f>
+          </x14:formula1>
+          <xm:sqref>D51</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$99</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$99</xm:f>
+          </x14:formula1>
+          <xm:sqref>D33:D37</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$99</xm:f>
+          </x14:formula1>
+          <xm:sqref>D18:D31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1720,7 +1764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed Tramsmittals-Send objectType to button.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1098,7 +1098,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1320,7 +1320,7 @@
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
         <v>56</v>

</xml_diff>